<commit_message>
Dummy First Record in All Excel Files
</commit_message>
<xml_diff>
--- a/src/assets/samples/CatalogProductMappingApprove.xlsx
+++ b/src/assets/samples/CatalogProductMappingApprove.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -89,16 +89,30 @@
   </si>
   <si>
     <t xml:space="preserve">IsApproved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1a2b3c4d5e-1234-1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dummy Catalog Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dummy Product Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIXED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY\ HH:MM"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -121,13 +135,26 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -164,12 +191,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -182,6 +225,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -190,25 +293,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1"/>
+  <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V1" activeCellId="0" sqref="V1"/>
+      <selection pane="topLeft" activeCell="X2" activeCellId="0" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="20.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="20.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.47"/>
@@ -296,6 +397,79 @@
       </c>
       <c r="AMJ1" s="0"/>
     </row>
+    <row r="2" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>-693594.531493056</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>-693594.531493056</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" s="4" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>